<commit_message>
update status and due date after sync from jira
</commit_message>
<xml_diff>
--- a/web/media/breakdown/IPROS-255/Breakdown-IPROS-255.xlsx
+++ b/web/media/breakdown/IPROS-255/Breakdown-IPROS-255.xlsx
@@ -49,7 +49,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -64,32 +64,11 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
@@ -97,8 +76,6 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -399,7 +376,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:E8"/>
+  <dimension ref="B2:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -409,8 +386,8 @@
   <cols>
     <col customWidth="1" max="1" min="1" width="2"/>
     <col customWidth="1" max="2" min="2" width="5"/>
-    <col customWidth="1" max="3" min="3" width="15"/>
-    <col customWidth="1" max="4" min="4" width="80"/>
+    <col customWidth="1" max="3" min="3" width="28"/>
+    <col customWidth="1" max="4" min="4" width="70"/>
     <col customWidth="1" max="5" min="5" width="15"/>
   </cols>
   <sheetData>
@@ -442,12 +419,12 @@
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>Summary of Changes</t>
+          <t>Details of Changes</t>
         </is>
       </c>
       <c r="D3" s="2" t="n"/>
       <c r="E3" s="2" t="n">
-        <v>0</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="4">
@@ -459,55 +436,22 @@
           <t>Other Impact</t>
         </is>
       </c>
-      <c r="D4" s="2" t="n"/>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Static Data Configurations Impact</t>
+        </is>
+      </c>
       <c r="E4" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="2" t="n"/>
-      <c r="E5" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="C6" s="4" t="n"/>
-      <c r="D6" s="2" t="n"/>
-      <c r="E6" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="inlineStr">
-        <is>
-          <t>Others</t>
-        </is>
-      </c>
-      <c r="D7" s="2" t="n"/>
-      <c r="E7" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="E8" s="5">
-        <f>SUM(F2:F7)</f>
+      <c r="E5" s="3">
+        <f>SUM(E2:E4)</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C4:C6"/>
-  </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>